<commit_message>
1. Model Pattern 세팅이 "Power" 항목 추가  - Power 설정이 ON 일 경우 Power Measure 후  Summary Log에 VCC, ICC 값 기록하도록 수정
</commit_message>
<xml_diff>
--- a/(VH)H1 NK향 BA검사기 SW 수정 History.xlsx
+++ b/(VH)H1 NK향 BA검사기 SW 수정 History.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="71">
   <si>
     <t>Site</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -253,10 +253,6 @@
   </si>
   <si>
     <t>GIE_BoadAssy_20230823_R1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GIE_BoadAssy_20230704_R1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -282,17 +278,30 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>GIE_BoadAssy_20230712_R1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GIE_BoadAssy_20230722_R1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1. LVDS FPGA, DP FPGA 버전 정보가 같은 버전값으로 표시되는 문제점 수정
  - Signal Type이 LVDS이면 LVDS FPGA에만, DP이면 DP FPGA에만 버전정보 표시.
  - Signal Type 설정에 따라 FPGA Module 전원 차단되기 때문에 둘다 동시에 표시하는 기능은 지원 불가.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Model Pattern 세팅이 "Power" 항목 추가
+ - Power 설정이 ON 일 경우 Power Measure 후  Summary Log에 VCC, ICC 값 기록하도록 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GIE_BoadAssy_20240704_R1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GIE_BoadAssy_20240712_R1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GIE_BoadAssy_20240722_R1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GIE_BoadAssy_20240801_R1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -898,7 +907,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>5914160</xdr:colOff>
@@ -928,6 +937,49 @@
         <a:xfrm>
           <a:off x="9646228" y="11785021"/>
           <a:ext cx="342986" cy="251115"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5792466</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>6398402</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>352426</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9526266" y="13249276"/>
+          <a:ext cx="605936" cy="209550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1210,10 +1262,10 @@
   <dimension ref="B1:K311"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G40" sqref="G40"/>
+      <selection pane="bottomRight" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2262,7 +2314,7 @@
         <v>45477</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6" t="s">
@@ -2270,7 +2322,7 @@
       </c>
       <c r="J38" s="7"/>
       <c r="K38" s="6" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="2:11" ht="24.75" customHeight="1">
@@ -2290,7 +2342,7 @@
         <v>45485</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6" t="s">
@@ -2298,7 +2350,7 @@
       </c>
       <c r="J39" s="7"/>
       <c r="K39" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="2:11" ht="47.25" customHeight="1">
@@ -2318,7 +2370,7 @@
         <v>45495</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H40" s="6"/>
       <c r="I40" s="6" t="s">
@@ -2326,20 +2378,36 @@
       </c>
       <c r="J40" s="7"/>
       <c r="K40" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" ht="24.75" customHeight="1">
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="1"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" ht="33" customHeight="1">
+      <c r="B41" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="5">
+        <v>45505</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="H41" s="6"/>
-      <c r="I41" s="8"/>
+      <c r="I41" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="J41" s="7"/>
-      <c r="K41" s="6"/>
+      <c r="K41" s="6" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="42" spans="2:11" ht="24.75" customHeight="1">
       <c r="B42" s="6"/>

</xml_diff>

<commit_message>
1. 9.9", 17" 모델 대응을 위한 PWM Setting 기능 추가  - Power Sequence에 PWM 항목 추가 및 PWM Freq, PWM Duty 설정 UI 추가
</commit_message>
<xml_diff>
--- a/(VH)H1 NK향 BA검사기 SW 수정 History.xlsx
+++ b/(VH)H1 NK향 BA검사기 SW 수정 History.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="73">
   <si>
     <t>Site</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -302,6 +302,15 @@
   </si>
   <si>
     <t>GIE_BoadAssy_20240801_R1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GIE_BoadAssy_20240920_R1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 9.9", 17" 모델 대응을 위한 PWM Setting 기능 추가
+ - Power Sequence에 PWM 항목 추가 및 PWM Freq, PWM Duty 설정 UI 추가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1262,10 +1271,10 @@
   <dimension ref="B1:K311"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G41" sqref="G41"/>
+      <selection pane="bottomRight" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2409,17 +2418,33 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="2:11" ht="24.75" customHeight="1">
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="7"/>
+    <row r="42" spans="2:11" ht="34.5" customHeight="1">
+      <c r="B42" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="5">
+        <v>45555</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
+      <c r="I42" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="J42" s="7"/>
-      <c r="K42" s="6"/>
+      <c r="K42" s="6" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="43" spans="2:11" ht="24.75" customHeight="1">
       <c r="B43" s="6"/>

</xml_diff>

<commit_message>
1. 20.5인치 모델 대응 Pixel Type "TRIPLE" 추가 2. 모델 Fusing 시 사용하지 않는 전압/전류 Limit 값 Low=0, High=99 고정값으로 Fusing 하도록 수정 3. Debug MLog 옵션 추가
</commit_message>
<xml_diff>
--- a/(VH)H1 NK향 BA검사기 SW 수정 History.xlsx
+++ b/(VH)H1 NK향 BA검사기 SW 수정 History.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="81">
   <si>
     <t>Site</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -328,6 +328,21 @@
   </si>
   <si>
     <t>1. Summary Log 기록후 초기화 하도록 수정 (M/C전 Model의 Pattern List가 기록되는 현상 수정)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 20.5인치 모델 대응 Pixel Type "TRIPLE" 추가</t>
+  </si>
+  <si>
+    <t>GIE_BoadAssy_20250522</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. System 메뉴에 Debug MLog 옵션 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GIE_BoadAssy_20250701</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1288,10 +1303,10 @@
   <dimension ref="B1:K311"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G44" sqref="G44"/>
+      <selection pane="bottomRight" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2520,28 +2535,60 @@
       </c>
     </row>
     <row r="45" spans="2:11" ht="24.75" customHeight="1">
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="7"/>
+      <c r="B45" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="5">
+        <v>45799</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
+      <c r="I45" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="J45" s="7"/>
-      <c r="K45" s="6"/>
+      <c r="K45" s="6" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="46" spans="2:11" ht="24.75" customHeight="1">
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="7"/>
+      <c r="B46" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="5">
+        <v>45839</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
+      <c r="I46" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="J46" s="7"/>
-      <c r="K46" s="6"/>
+      <c r="K46" s="6" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="47" spans="2:11" ht="24.75" customHeight="1">
       <c r="B47" s="6"/>

</xml_diff>